<commit_message>
Updated the physical model and the Database spreedsheet
</commit_message>
<xml_diff>
--- a/OlympicGamesApp_Database.xlsx
+++ b/OlympicGamesApp_Database.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="163">
   <si>
     <t>Country</t>
   </si>
@@ -95,9 +95,6 @@
     <t>FavoriteCountry</t>
   </si>
   <si>
-    <t>UserId</t>
-  </si>
-  <si>
     <t>FirstName</t>
   </si>
   <si>
@@ -216,6 +213,306 @@
   </si>
   <si>
     <t>kenling@hotmail.com</t>
+  </si>
+  <si>
+    <t>PurchaseDate</t>
+  </si>
+  <si>
+    <t>TotalCost</t>
+  </si>
+  <si>
+    <t>TicketOrder</t>
+  </si>
+  <si>
+    <t>TicketOrderId</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>TotalItemPrice</t>
+  </si>
+  <si>
+    <t>TicketOrderItem</t>
+  </si>
+  <si>
+    <t>TicketEventId</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>TicketPrice</t>
+  </si>
+  <si>
+    <t>TicketsAvailable</t>
+  </si>
+  <si>
+    <t>VenueSectorId</t>
+  </si>
+  <si>
+    <t>TicketEvent</t>
+  </si>
+  <si>
+    <t>AthleteId</t>
+  </si>
+  <si>
+    <t>FavoriteSport</t>
+  </si>
+  <si>
+    <t>SportId</t>
+  </si>
+  <si>
+    <t>FavoriteModality</t>
+  </si>
+  <si>
+    <t>ModalityId</t>
+  </si>
+  <si>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>Swimming</t>
+  </si>
+  <si>
+    <t>Basketball</t>
+  </si>
+  <si>
+    <t>Tennis</t>
+  </si>
+  <si>
+    <t>Judo</t>
+  </si>
+  <si>
+    <t>AthleteModality</t>
+  </si>
+  <si>
+    <t>ModalityCategory</t>
+  </si>
+  <si>
+    <t>Individual</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>Modality</t>
+  </si>
+  <si>
+    <t>ModalityCategoryId</t>
+  </si>
+  <si>
+    <t>men 100m freestyle</t>
+  </si>
+  <si>
+    <t>men 200m freestyle</t>
+  </si>
+  <si>
+    <t>men 4x100m medley</t>
+  </si>
+  <si>
+    <t>men tennis double</t>
+  </si>
+  <si>
+    <t>men tennis single</t>
+  </si>
+  <si>
+    <t>men basketball</t>
+  </si>
+  <si>
+    <t>CompetitionSession</t>
+  </si>
+  <si>
+    <t>CompetitionPhase</t>
+  </si>
+  <si>
+    <t>Preliminary</t>
+  </si>
+  <si>
+    <t>FirstRound</t>
+  </si>
+  <si>
+    <t>SecondRound</t>
+  </si>
+  <si>
+    <t>ThirdRound</t>
+  </si>
+  <si>
+    <t>Quarters</t>
+  </si>
+  <si>
+    <t>Semi Finals</t>
+  </si>
+  <si>
+    <t>Finals</t>
+  </si>
+  <si>
+    <t>Heats</t>
+  </si>
+  <si>
+    <t>men 66-73kg (lightweight)</t>
+  </si>
+  <si>
+    <t>Repechage</t>
+  </si>
+  <si>
+    <t>Bronze match</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>AdressStreet</t>
+  </si>
+  <si>
+    <t>Venue</t>
+  </si>
+  <si>
+    <t>Aquatic Olympic Statium</t>
+  </si>
+  <si>
+    <t>Juventude Arena</t>
+  </si>
+  <si>
+    <t>Carioca Arena</t>
+  </si>
+  <si>
+    <t>Tennis Olympic Center</t>
+  </si>
+  <si>
+    <t>Barra</t>
+  </si>
+  <si>
+    <t>Botafogo</t>
+  </si>
+  <si>
+    <t>Flamengo</t>
+  </si>
+  <si>
+    <t>Copacabana</t>
+  </si>
+  <si>
+    <t>RJ</t>
+  </si>
+  <si>
+    <t>R Mal. Floriano 234</t>
+  </si>
+  <si>
+    <t>R. Mal Deodoro 658</t>
+  </si>
+  <si>
+    <t>Av. Iguacu 345</t>
+  </si>
+  <si>
+    <t>Av. Brasil 23</t>
+  </si>
+  <si>
+    <t>CompetitionEventTicket</t>
+  </si>
+  <si>
+    <t>CompetitionEventId</t>
+  </si>
+  <si>
+    <t>CompetitionSessionId</t>
+  </si>
+  <si>
+    <t>CompetitionPhaseId</t>
+  </si>
+  <si>
+    <t>VenueId</t>
+  </si>
+  <si>
+    <t>BasePrice</t>
+  </si>
+  <si>
+    <t>CompetitionEvent</t>
+  </si>
+  <si>
+    <t>Session 10</t>
+  </si>
+  <si>
+    <t>Session 22</t>
+  </si>
+  <si>
+    <t>Session 25</t>
+  </si>
+  <si>
+    <t>Session 38</t>
+  </si>
+  <si>
+    <t>Session 8</t>
+  </si>
+  <si>
+    <t>Session 9</t>
+  </si>
+  <si>
+    <t>Session 2</t>
+  </si>
+  <si>
+    <t>Session 4</t>
+  </si>
+  <si>
+    <t>Session 3</t>
+  </si>
+  <si>
+    <t>Session 1</t>
+  </si>
+  <si>
+    <t>FavoriteAthlete</t>
+  </si>
+  <si>
+    <t>Multiplier</t>
+  </si>
+  <si>
+    <t>VenueSector</t>
+  </si>
+  <si>
+    <t>SectorA</t>
+  </si>
+  <si>
+    <t>SectorB</t>
+  </si>
+  <si>
+    <t>SectorC</t>
+  </si>
+  <si>
+    <t>SectorD</t>
+  </si>
+  <si>
+    <t>Sector A</t>
+  </si>
+  <si>
+    <t>Sector B</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>06/08/2016 - 14:00 - Men Basketball Preliminary Session 1</t>
+  </si>
+  <si>
+    <t>CustomerId</t>
+  </si>
+  <si>
+    <t>21/08/2016 - 15:00 - Men Basketball Finals Session 38</t>
+  </si>
+  <si>
+    <t>07/08/2016 - 11:00 - Men 100m freestyle Finals Session 10</t>
+  </si>
+  <si>
+    <t>Lleyton</t>
+  </si>
+  <si>
+    <t>Hewitt</t>
+  </si>
+  <si>
+    <t>13/08/2016 - 11:00 - Men 4x100m medley Finals Session 10</t>
+  </si>
+  <si>
+    <t>09/08/2016 - 10:00 - Men tennis single Finals Session 22</t>
   </si>
 </sst>
 </file>
@@ -231,15 +528,33 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -421,11 +736,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -448,31 +800,100 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -755,32 +1176,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AD14"/>
+  <dimension ref="A1:AD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P15" sqref="P15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y45" sqref="Y45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="2.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="9.140625" style="1"/>
+    <col min="12" max="12" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="9.28515625" style="1" customWidth="1"/>
     <col min="17" max="17" width="4.7109375" style="1" customWidth="1"/>
-    <col min="18" max="18" width="10.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.28515625" style="1" customWidth="1"/>
     <col min="19" max="19" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="14.28515625" style="1" customWidth="1"/>
     <col min="22" max="22" width="9.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="14.28515625" style="1" bestFit="1" customWidth="1"/>
@@ -794,123 +1218,123 @@
   <sheetData>
     <row r="1" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="11"/>
-      <c r="M2" s="10" t="s">
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="28"/>
+      <c r="M2" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="11"/>
-      <c r="Q2" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="R2" s="15"/>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="11"/>
+      <c r="N2" s="28"/>
+      <c r="Q2" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="R2" s="27"/>
+      <c r="S2" s="27"/>
+      <c r="T2" s="27"/>
+      <c r="U2" s="27"/>
+      <c r="V2" s="27"/>
+      <c r="W2" s="27"/>
+      <c r="X2" s="27"/>
+      <c r="Y2" s="27"/>
+      <c r="Z2" s="27"/>
+      <c r="AA2" s="27"/>
+      <c r="AB2" s="27"/>
+      <c r="AC2" s="27"/>
+      <c r="AD2" s="28"/>
     </row>
     <row r="3" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="16" t="s">
+      <c r="B3" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="11"/>
-      <c r="M3" s="8" t="s">
+      <c r="H3" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="28"/>
+      <c r="M3" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="N3" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q3" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="N3" s="9" t="s">
+      <c r="S3" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="T3" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="V3" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="W3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Y3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="Z3" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA3" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="Q3" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="R3" s="16" t="s">
-        <v>24</v>
-      </c>
-      <c r="S3" s="16" t="s">
-        <v>9</v>
-      </c>
-      <c r="T3" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="U3" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="V3" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="W3" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="X3" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="Y3" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="Z3" s="16" t="s">
+      <c r="AB3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="AA3" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB3" s="16" t="s">
+      <c r="AC3" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="AC3" s="16" t="s">
+      <c r="AD3" s="8" t="s">
         <v>30</v>
-      </c>
-      <c r="AD3" s="9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="14">
-        <v>2</v>
-      </c>
-      <c r="E4" s="14">
+      <c r="C4" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="12">
+        <v>2</v>
+      </c>
+      <c r="E4" s="12">
         <v>3</v>
       </c>
       <c r="F4" s="7">
         <v>1</v>
       </c>
-      <c r="H4" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" s="9" t="s">
+      <c r="H4" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>2</v>
       </c>
       <c r="M4" s="6">
@@ -922,58 +1346,58 @@
       <c r="Q4" s="6">
         <v>1</v>
       </c>
-      <c r="R4" s="14" t="s">
+      <c r="R4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="S4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="S4" s="14" t="s">
+      <c r="T4" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="T4" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="U4" s="14">
+      <c r="U4" s="12">
         <v>34</v>
       </c>
-      <c r="V4" s="14">
-        <v>1</v>
-      </c>
-      <c r="W4" s="14" t="s">
+      <c r="V4" s="12">
+        <v>1</v>
+      </c>
+      <c r="W4" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="X4" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="X4" s="14" t="s">
+      <c r="Y4" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="Y4" s="14" t="s">
+      <c r="Z4" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="Z4" s="14" t="s">
+      <c r="AA4" s="12">
+        <v>3</v>
+      </c>
+      <c r="AB4" s="12">
+        <v>2099</v>
+      </c>
+      <c r="AC4" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="AA4" s="14">
-        <v>3</v>
-      </c>
-      <c r="AB4" s="14">
-        <v>2099</v>
-      </c>
-      <c r="AC4" s="14" t="s">
+      <c r="AD4" s="7" t="s">
         <v>44</v>
-      </c>
-      <c r="AD4" s="7" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
         <v>2</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="14">
-        <v>2</v>
-      </c>
-      <c r="E5" s="14">
-        <v>1</v>
+      <c r="D5" s="12">
+        <v>2</v>
+      </c>
+      <c r="E5" s="12">
+        <v>2</v>
       </c>
       <c r="F5" s="7">
         <v>1</v>
@@ -982,7 +1406,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M5" s="2">
         <v>1</v>
@@ -993,57 +1417,57 @@
       <c r="Q5" s="2">
         <v>2</v>
       </c>
-      <c r="R5" s="12" t="s">
+      <c r="R5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="S5" s="12" t="s">
+      <c r="T5" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="U5" s="10">
+        <v>57</v>
+      </c>
+      <c r="V5" s="10">
+        <v>2</v>
+      </c>
+      <c r="W5" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="T5" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="U5" s="12">
-        <v>57</v>
-      </c>
-      <c r="V5" s="12">
-        <v>2</v>
-      </c>
-      <c r="W5" s="12" t="s">
+      <c r="X5" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="X5" s="12" t="s">
+      <c r="Y5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="Y5" s="12" t="s">
+      <c r="Z5" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="Z5" s="12" t="s">
+      <c r="AA5" s="10">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="10">
+        <v>81280270</v>
+      </c>
+      <c r="AC5" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="AA5" s="12">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="12">
-        <v>81280270</v>
-      </c>
-      <c r="AC5" s="12" t="s">
+      <c r="AD5" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="AD5" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2">
         <v>3</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="12">
-        <v>1</v>
-      </c>
-      <c r="E6" s="12">
+      <c r="D6" s="10">
+        <v>2</v>
+      </c>
+      <c r="E6" s="10">
         <v>2</v>
       </c>
       <c r="F6" s="3">
@@ -1053,68 +1477,68 @@
         <v>2</v>
       </c>
       <c r="I6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6" s="2">
+        <v>2</v>
+      </c>
+      <c r="N6" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="4">
+        <v>3</v>
+      </c>
+      <c r="R6" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="T6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="U6" s="11">
         <v>38</v>
       </c>
-      <c r="M6" s="2">
-        <v>2</v>
-      </c>
-      <c r="N6" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="4">
-        <v>3</v>
-      </c>
-      <c r="R6" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="S6" s="13" t="s">
+      <c r="V6" s="11">
+        <v>1</v>
+      </c>
+      <c r="W6" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="T6" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="U6" s="13">
-        <v>38</v>
-      </c>
-      <c r="V6" s="13">
-        <v>1</v>
-      </c>
-      <c r="W6" s="13" t="s">
+      <c r="X6" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y6" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="X6" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="Y6" s="13" t="s">
+      <c r="Z6" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="Z6" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="AA6" s="13">
+      <c r="AA6" s="11">
         <v>4</v>
       </c>
-      <c r="AB6" s="13">
+      <c r="AB6" s="11">
         <v>43000</v>
       </c>
-      <c r="AC6" s="13" t="s">
-        <v>63</v>
+      <c r="AC6" s="11" t="s">
+        <v>62</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="4">
         <v>4</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="D7" s="13">
+      <c r="C7" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D7" s="11">
         <v>0</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="11">
         <v>2</v>
       </c>
       <c r="F7" s="5">
@@ -1127,150 +1551,1518 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M9" s="26" t="s">
+        <v>145</v>
+      </c>
+      <c r="N9" s="28"/>
+      <c r="Q9" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="R9" s="27"/>
+      <c r="S9" s="27"/>
+      <c r="T9" s="28"/>
+    </row>
     <row r="10" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="11"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="27"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="28"/>
+      <c r="M10" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="N10" s="38" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q10" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="R10" s="36" t="s">
+        <v>156</v>
+      </c>
+      <c r="S10" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="T10" s="9" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="11" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C11" s="16" t="s">
+      <c r="B11" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="H11" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="I11" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="J11" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="K11" s="9" t="s">
+      <c r="K11" s="15" t="s">
         <v>7</v>
+      </c>
+      <c r="M11" s="6">
+        <v>1</v>
+      </c>
+      <c r="N11" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>1</v>
+      </c>
+      <c r="R11" s="12">
+        <v>1</v>
+      </c>
+      <c r="S11" s="18">
+        <v>42495</v>
+      </c>
+      <c r="T11" s="7">
+        <f>U19+U20+U21</f>
+        <v>2476.5</v>
       </c>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>1</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14" t="s">
+      <c r="D12" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="F12" s="14">
+      <c r="F12" s="12">
         <v>25</v>
       </c>
-      <c r="G12" s="14">
-        <v>1</v>
-      </c>
-      <c r="H12" s="14">
-        <v>2</v>
-      </c>
-      <c r="I12" s="14">
-        <v>2</v>
-      </c>
-      <c r="J12" s="14">
-        <v>1</v>
+      <c r="G12" s="12">
+        <v>1</v>
+      </c>
+      <c r="H12" s="12">
+        <v>2</v>
+      </c>
+      <c r="I12" s="12">
+        <v>2</v>
+      </c>
+      <c r="J12" s="12">
+        <v>2</v>
       </c>
       <c r="K12" s="7">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:30" x14ac:dyDescent="0.25">
+      <c r="M12" s="2">
+        <v>1</v>
+      </c>
+      <c r="N12" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q12" s="2">
+        <v>2</v>
+      </c>
+      <c r="R12" s="10">
+        <v>2</v>
+      </c>
+      <c r="S12" s="16">
+        <v>42498</v>
+      </c>
+      <c r="T12" s="3">
+        <f>U22</f>
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="13" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2">
         <v>2</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12" t="s">
+      <c r="D13" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="12">
+      <c r="F13" s="10">
         <v>28</v>
       </c>
-      <c r="G13" s="12">
-        <v>1</v>
-      </c>
-      <c r="H13" s="12">
-        <v>3</v>
-      </c>
-      <c r="I13" s="12">
-        <v>1</v>
-      </c>
-      <c r="J13" s="12">
+      <c r="G13" s="10">
+        <v>1</v>
+      </c>
+      <c r="H13" s="10">
+        <v>3</v>
+      </c>
+      <c r="I13" s="10">
+        <v>1</v>
+      </c>
+      <c r="J13" s="10">
         <v>2</v>
       </c>
       <c r="K13" s="3">
         <v>1</v>
       </c>
+      <c r="M13" s="2">
+        <v>2</v>
+      </c>
+      <c r="N13" s="3">
+        <v>4</v>
+      </c>
+      <c r="Q13" s="4">
+        <v>3</v>
+      </c>
+      <c r="R13" s="11">
+        <v>3</v>
+      </c>
+      <c r="S13" s="17">
+        <v>42501</v>
+      </c>
+      <c r="T13" s="5">
+        <f>U23</f>
+        <v>1008</v>
+      </c>
     </row>
     <row r="14" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="4">
-        <v>3</v>
-      </c>
-      <c r="C14" s="13" t="s">
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F14" s="10">
+        <v>34</v>
+      </c>
+      <c r="G14" s="10">
+        <v>1</v>
+      </c>
+      <c r="H14" s="10">
+        <v>3</v>
+      </c>
+      <c r="I14" s="10">
+        <v>1</v>
+      </c>
+      <c r="J14" s="10">
+        <v>0</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="M14" s="4">
+        <v>3</v>
+      </c>
+      <c r="N14" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="4">
+        <v>4</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13" t="s">
+      <c r="D15" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F14" s="13">
+      <c r="F15" s="11">
         <v>24</v>
       </c>
-      <c r="G14" s="13">
-        <v>1</v>
-      </c>
-      <c r="H14" s="13">
-        <v>1</v>
-      </c>
-      <c r="I14" s="13">
-        <v>2</v>
-      </c>
-      <c r="J14" s="13">
-        <v>3</v>
-      </c>
-      <c r="K14" s="5">
-        <v>1</v>
+      <c r="G15" s="11">
+        <v>1</v>
+      </c>
+      <c r="H15" s="11">
+        <v>1</v>
+      </c>
+      <c r="I15" s="11">
+        <v>2</v>
+      </c>
+      <c r="J15" s="11">
+        <v>3</v>
+      </c>
+      <c r="K15" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="28"/>
+      <c r="E17" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="F17" s="28"/>
+      <c r="H17" s="26" t="s">
+        <v>87</v>
+      </c>
+      <c r="I17" s="28"/>
+      <c r="M17" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="N17" s="28"/>
+      <c r="Q17" s="29" t="s">
+        <v>69</v>
+      </c>
+      <c r="R17" s="30"/>
+      <c r="S17" s="30"/>
+      <c r="T17" s="30"/>
+      <c r="U17" s="31"/>
+    </row>
+    <row r="18" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="37" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="N18" s="38" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q18" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" s="36" t="s">
+        <v>70</v>
+      </c>
+      <c r="S18" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="T18" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="U18" s="15" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B19" s="6">
+        <v>1</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="E19" s="6">
+        <v>1</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="H19" s="6">
+        <v>1</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="M19" s="6">
+        <v>1</v>
+      </c>
+      <c r="N19" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="6">
+        <v>1</v>
+      </c>
+      <c r="R19" s="12">
+        <v>1</v>
+      </c>
+      <c r="S19" s="12">
+        <v>1</v>
+      </c>
+      <c r="T19" s="12">
+        <v>3</v>
+      </c>
+      <c r="U19" s="7">
+        <f>S27*T19</f>
+        <v>136.5</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
+        <v>2</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="2">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3">
+        <v>2</v>
+      </c>
+      <c r="H20" s="4">
+        <v>2</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="M20" s="2">
+        <v>1</v>
+      </c>
+      <c r="N20" s="3">
+        <v>2</v>
+      </c>
+      <c r="Q20" s="2">
+        <v>2</v>
+      </c>
+      <c r="R20" s="10">
+        <v>2</v>
+      </c>
+      <c r="S20" s="10">
+        <v>1</v>
+      </c>
+      <c r="T20" s="10">
+        <v>5</v>
+      </c>
+      <c r="U20" s="3">
+        <f>S28*T20</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="2">
+        <v>3</v>
+      </c>
+      <c r="F21" s="3">
+        <v>1</v>
+      </c>
+      <c r="M21" s="2">
+        <v>2</v>
+      </c>
+      <c r="N21" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="2">
+        <v>3</v>
+      </c>
+      <c r="R21" s="10">
+        <v>3</v>
+      </c>
+      <c r="S21" s="10">
+        <v>1</v>
+      </c>
+      <c r="T21" s="10">
+        <v>4</v>
+      </c>
+      <c r="U21" s="3">
+        <f>S29*T21</f>
+        <v>1440</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="4">
+        <v>4</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="4">
+        <v>3</v>
+      </c>
+      <c r="F22" s="5">
+        <v>3</v>
+      </c>
+      <c r="M22" s="4">
+        <v>3</v>
+      </c>
+      <c r="N22" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q22" s="2">
+        <v>4</v>
+      </c>
+      <c r="R22" s="10">
+        <v>4</v>
+      </c>
+      <c r="S22" s="10">
+        <v>2</v>
+      </c>
+      <c r="T22" s="10">
+        <v>8</v>
+      </c>
+      <c r="U22" s="3">
+        <f>S30*T22</f>
+        <v>2160</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q23" s="4">
+        <v>5</v>
+      </c>
+      <c r="R23" s="11">
+        <v>5</v>
+      </c>
+      <c r="S23" s="11">
+        <v>3</v>
+      </c>
+      <c r="T23" s="11">
+        <v>7</v>
+      </c>
+      <c r="U23" s="5">
+        <f>S31*T23</f>
+        <v>1008</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="25" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C25" s="27"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="28"/>
+      <c r="G25" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="H25" s="28"/>
+      <c r="J25" s="26" t="s">
+        <v>99</v>
+      </c>
+      <c r="K25" s="28"/>
+      <c r="Q25" s="29" t="s">
+        <v>75</v>
+      </c>
+      <c r="R25" s="30"/>
+      <c r="S25" s="30"/>
+      <c r="T25" s="30"/>
+      <c r="U25" s="31"/>
+    </row>
+    <row r="26" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="36" t="s">
+        <v>91</v>
+      </c>
+      <c r="E26" s="39" t="s">
+        <v>78</v>
+      </c>
+      <c r="G26" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M26" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="N26" s="31"/>
+      <c r="Q26" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="R26" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="S26" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="T26" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="U26" s="39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="6">
+        <v>1</v>
+      </c>
+      <c r="C27" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="D27" s="12">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6">
+        <v>1</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="J27" s="6">
+        <v>1</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="M27" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="N27" s="38" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q27" s="6">
+        <v>1</v>
+      </c>
+      <c r="R27" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="S27" s="12">
+        <f>O47*D49</f>
+        <v>45.5</v>
+      </c>
+      <c r="T27" s="12">
+        <v>19997</v>
+      </c>
+      <c r="U27" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>2</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D28" s="10">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2">
+        <v>2</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J28" s="2">
+        <v>2</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M28" s="6">
+        <v>1</v>
+      </c>
+      <c r="N28" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>2</v>
+      </c>
+      <c r="R28" s="33" t="s">
+        <v>157</v>
+      </c>
+      <c r="S28" s="32">
+        <f>O48*D50</f>
+        <v>180</v>
+      </c>
+      <c r="T28" s="10">
+        <v>19995</v>
+      </c>
+      <c r="U28" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>3</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="D29" s="10">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <v>3</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="J29" s="2">
+        <v>3</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="M29" s="2">
+        <v>1</v>
+      </c>
+      <c r="N29" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>3</v>
+      </c>
+      <c r="R29" s="33" t="s">
+        <v>158</v>
+      </c>
+      <c r="S29" s="10">
+        <f>O54*D54</f>
+        <v>360</v>
+      </c>
+      <c r="T29" s="10">
+        <v>19996</v>
+      </c>
+      <c r="U29" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>4</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D30" s="10">
+        <v>1</v>
+      </c>
+      <c r="E30" s="3">
+        <v>3</v>
+      </c>
+      <c r="G30" s="2">
+        <v>4</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J30" s="2">
+        <v>4</v>
+      </c>
+      <c r="K30" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="M30" s="2">
+        <v>2</v>
+      </c>
+      <c r="N30" s="3">
+        <v>3</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>4</v>
+      </c>
+      <c r="R30" s="33" t="s">
+        <v>161</v>
+      </c>
+      <c r="S30" s="10">
+        <f>O56*D53</f>
+        <v>270</v>
+      </c>
+      <c r="T30" s="10">
+        <v>19992</v>
+      </c>
+      <c r="U30" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="2">
+        <v>5</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="D31" s="10">
+        <v>2</v>
+      </c>
+      <c r="E31" s="3">
+        <v>3</v>
+      </c>
+      <c r="G31" s="2">
+        <v>5</v>
+      </c>
+      <c r="H31" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="J31" s="2">
+        <v>5</v>
+      </c>
+      <c r="K31" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="M31" s="4">
+        <v>3</v>
+      </c>
+      <c r="N31" s="5">
+        <v>4</v>
+      </c>
+      <c r="Q31" s="4">
+        <v>5</v>
+      </c>
+      <c r="R31" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="S31" s="11">
+        <f>O55*D56</f>
+        <v>144</v>
+      </c>
+      <c r="T31" s="11">
+        <v>19993</v>
+      </c>
+      <c r="U31" s="5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <v>6</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="D32" s="10">
+        <v>1</v>
+      </c>
+      <c r="E32" s="3">
+        <v>4</v>
+      </c>
+      <c r="G32" s="2">
+        <v>6</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="J32" s="2">
+        <v>6</v>
+      </c>
+      <c r="K32" s="3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="4">
+        <v>7</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="11">
+        <v>2</v>
+      </c>
+      <c r="E33" s="5">
+        <v>2</v>
+      </c>
+      <c r="G33" s="2">
+        <v>7</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="J33" s="2">
+        <v>7</v>
+      </c>
+      <c r="K33" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G34" s="2">
+        <v>8</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="J34" s="2">
+        <v>8</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M34" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="N34" s="28"/>
+    </row>
+    <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G35" s="2">
+        <v>9</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="J35" s="2">
+        <v>9</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="M35" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="N35" s="38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G36" s="4">
+        <v>10</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="J36" s="4">
+        <v>10</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="M36" s="6">
+        <v>1</v>
+      </c>
+      <c r="N36" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M37" s="2">
+        <v>2</v>
+      </c>
+      <c r="N37" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="26" t="s">
+        <v>114</v>
+      </c>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="28"/>
+      <c r="M38" s="2">
+        <v>8</v>
+      </c>
+      <c r="N38" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E39" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F39" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M39" s="2">
+        <v>10</v>
+      </c>
+      <c r="N39" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B40" s="6">
+        <v>1</v>
+      </c>
+      <c r="C40" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="D40" s="12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F40" s="12">
+        <v>64585269</v>
+      </c>
+      <c r="G40" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="M40" s="4">
+        <v>9</v>
+      </c>
+      <c r="N40" s="5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="2">
+        <v>2</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="E41" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="F41" s="10">
+        <v>63348684</v>
+      </c>
+      <c r="G41" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="2">
+        <v>3</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D42" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="E42" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F42" s="10">
+        <v>69484131</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B43" s="4">
+        <v>4</v>
+      </c>
+      <c r="C43" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="F43" s="11">
+        <v>63215987</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H45" s="26" t="s">
+        <v>134</v>
+      </c>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="27"/>
+      <c r="M45" s="27"/>
+      <c r="N45" s="27"/>
+      <c r="O45" s="28"/>
+    </row>
+    <row r="46" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="26" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" s="27"/>
+      <c r="D46" s="27"/>
+      <c r="E46" s="28"/>
+      <c r="H46" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="I46" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="J46" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="K46" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="L46" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="M46" s="36" t="s">
+        <v>131</v>
+      </c>
+      <c r="N46" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="O46" s="9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E47" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="H47" s="6">
+        <v>1</v>
+      </c>
+      <c r="I47" s="18">
+        <v>42588</v>
+      </c>
+      <c r="J47" s="23">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="K47" s="12">
+        <v>7</v>
+      </c>
+      <c r="L47" s="12">
+        <v>1</v>
+      </c>
+      <c r="M47" s="12">
+        <v>2</v>
+      </c>
+      <c r="N47" s="12">
+        <v>2</v>
+      </c>
+      <c r="O47" s="24">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B48" s="6">
+        <v>1</v>
+      </c>
+      <c r="C48" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" s="12">
+        <v>1</v>
+      </c>
+      <c r="E48" s="7">
+        <v>2</v>
+      </c>
+      <c r="H48" s="2">
+        <v>2</v>
+      </c>
+      <c r="I48" s="16">
+        <v>42603</v>
+      </c>
+      <c r="J48" s="19">
+        <v>0.625</v>
+      </c>
+      <c r="K48" s="10">
+        <v>7</v>
+      </c>
+      <c r="L48" s="10">
+        <v>10</v>
+      </c>
+      <c r="M48" s="10">
+        <v>10</v>
+      </c>
+      <c r="N48" s="10">
+        <v>2</v>
+      </c>
+      <c r="O48" s="20">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B49" s="2">
+        <v>2</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D49" s="10">
+        <v>1.3</v>
+      </c>
+      <c r="E49" s="3">
+        <v>2</v>
+      </c>
+      <c r="H49" s="2">
+        <v>3</v>
+      </c>
+      <c r="I49" s="16">
+        <v>42588</v>
+      </c>
+      <c r="J49" s="19">
+        <v>0.375</v>
+      </c>
+      <c r="K49" s="10">
+        <v>1</v>
+      </c>
+      <c r="L49" s="10">
+        <v>1</v>
+      </c>
+      <c r="M49" s="10">
+        <v>1</v>
+      </c>
+      <c r="N49" s="10">
+        <v>3</v>
+      </c>
+      <c r="O49" s="20">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B50" s="2">
+        <v>3</v>
+      </c>
+      <c r="C50" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D50" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="E50" s="3">
+        <v>2</v>
+      </c>
+      <c r="H50" s="2">
+        <v>4</v>
+      </c>
+      <c r="I50" s="16">
+        <v>42588</v>
+      </c>
+      <c r="J50" s="19">
+        <v>0.3833333333333333</v>
+      </c>
+      <c r="K50" s="10">
+        <v>1</v>
+      </c>
+      <c r="L50" s="10">
+        <v>2</v>
+      </c>
+      <c r="M50" s="10">
+        <v>1</v>
+      </c>
+      <c r="N50" s="10">
+        <v>3</v>
+      </c>
+      <c r="O50" s="20">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B51" s="2">
+        <v>4</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D51" s="10">
+        <v>1.7</v>
+      </c>
+      <c r="E51" s="3">
+        <v>2</v>
+      </c>
+      <c r="H51" s="2">
+        <v>5</v>
+      </c>
+      <c r="I51" s="16">
+        <v>42588</v>
+      </c>
+      <c r="J51" s="19">
+        <v>0.39583333333333331</v>
+      </c>
+      <c r="K51" s="10">
+        <v>1</v>
+      </c>
+      <c r="L51" s="10">
+        <v>4</v>
+      </c>
+      <c r="M51" s="10">
+        <v>1</v>
+      </c>
+      <c r="N51" s="10">
+        <v>3</v>
+      </c>
+      <c r="O51" s="20">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B52" s="2">
+        <v>5</v>
+      </c>
+      <c r="C52" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" s="10">
+        <v>1</v>
+      </c>
+      <c r="E52" s="3">
+        <v>3</v>
+      </c>
+      <c r="H52" s="2">
+        <v>6</v>
+      </c>
+      <c r="I52" s="16">
+        <v>42588</v>
+      </c>
+      <c r="J52" s="19">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="K52" s="10">
+        <v>1</v>
+      </c>
+      <c r="L52" s="10">
+        <v>5</v>
+      </c>
+      <c r="M52" s="10">
+        <v>9</v>
+      </c>
+      <c r="N52" s="10">
+        <v>3</v>
+      </c>
+      <c r="O52" s="20">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B53" s="2">
+        <v>6</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D53" s="10">
+        <v>1.5</v>
+      </c>
+      <c r="E53" s="3">
+        <v>3</v>
+      </c>
+      <c r="H53" s="2">
+        <v>7</v>
+      </c>
+      <c r="I53" s="16">
+        <v>42588</v>
+      </c>
+      <c r="J53" s="19">
+        <v>0.67499999999999993</v>
+      </c>
+      <c r="K53" s="10">
+        <v>1</v>
+      </c>
+      <c r="L53" s="10">
+        <v>6</v>
+      </c>
+      <c r="M53" s="10">
+        <v>9</v>
+      </c>
+      <c r="N53" s="10">
+        <v>3</v>
+      </c>
+      <c r="O53" s="20">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B54" s="2">
+        <v>7</v>
+      </c>
+      <c r="C54" s="10" t="s">
+        <v>150</v>
+      </c>
+      <c r="D54" s="10">
+        <v>2</v>
+      </c>
+      <c r="E54" s="3">
+        <v>3</v>
+      </c>
+      <c r="H54" s="2">
+        <v>8</v>
+      </c>
+      <c r="I54" s="16">
+        <v>42589</v>
+      </c>
+      <c r="J54" s="19">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K54" s="10">
+        <v>1</v>
+      </c>
+      <c r="L54" s="10">
+        <v>7</v>
+      </c>
+      <c r="M54" s="10">
+        <v>10</v>
+      </c>
+      <c r="N54" s="10">
+        <v>3</v>
+      </c>
+      <c r="O54" s="20">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="55" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B55" s="2">
+        <v>8</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D55" s="10">
+        <v>1</v>
+      </c>
+      <c r="E55" s="3">
+        <v>4</v>
+      </c>
+      <c r="H55" s="2">
+        <v>9</v>
+      </c>
+      <c r="I55" s="16">
+        <v>42591</v>
+      </c>
+      <c r="J55" s="19">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="K55" s="10">
+        <v>4</v>
+      </c>
+      <c r="L55" s="10">
+        <v>8</v>
+      </c>
+      <c r="M55" s="10">
+        <v>10</v>
+      </c>
+      <c r="N55" s="10">
+        <v>4</v>
+      </c>
+      <c r="O55" s="20">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B56" s="4">
+        <v>9</v>
+      </c>
+      <c r="C56" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="D56" s="11">
+        <v>1.8</v>
+      </c>
+      <c r="E56" s="5">
+        <v>4</v>
+      </c>
+      <c r="H56" s="4">
+        <v>10</v>
+      </c>
+      <c r="I56" s="17">
+        <v>42595</v>
+      </c>
+      <c r="J56" s="21">
+        <v>0.45833333333333331</v>
+      </c>
+      <c r="K56" s="11">
+        <v>3</v>
+      </c>
+      <c r="L56" s="11">
+        <v>7</v>
+      </c>
+      <c r="M56" s="11">
+        <v>10</v>
+      </c>
+      <c r="N56" s="11">
+        <v>3</v>
+      </c>
+      <c r="O56" s="22">
+        <v>180</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="21">
+    <mergeCell ref="Q2:AD2"/>
+    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="Q9:T9"/>
+    <mergeCell ref="M9:N9"/>
+    <mergeCell ref="M17:N17"/>
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B10:K10"/>
     <mergeCell ref="M2:N2"/>
-    <mergeCell ref="Q2:AD2"/>
-    <mergeCell ref="H3:I3"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="Q17:U17"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="Q25:U25"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="B38:G38"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="H45:O45"/>
+    <mergeCell ref="M26:N26"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AC4" r:id="rId1"/>
@@ -1278,5 +3070,6 @@
     <hyperlink ref="AC6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Defined all the model classes, mapping and seeding database.
</commit_message>
<xml_diff>
--- a/OlympicGamesApp_Database.xlsx
+++ b/OlympicGamesApp_Database.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="180">
   <si>
     <t>Country</t>
   </si>
@@ -59,9 +60,6 @@
     <t>LastName</t>
   </si>
   <si>
-    <t>Age</t>
-  </si>
-  <si>
     <t>GenderId</t>
   </si>
   <si>
@@ -500,19 +498,73 @@
     <t>21/08/2016 - 15:00 - Men Basketball Finals Session 38</t>
   </si>
   <si>
-    <t>07/08/2016 - 11:00 - Men 100m freestyle Finals Session 10</t>
-  </si>
-  <si>
     <t>Lleyton</t>
   </si>
   <si>
     <t>Hewitt</t>
   </si>
   <si>
-    <t>13/08/2016 - 11:00 - Men 4x100m medley Finals Session 10</t>
-  </si>
-  <si>
     <t>09/08/2016 - 10:00 - Men tennis single Finals Session 22</t>
+  </si>
+  <si>
+    <t>DOB</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>CustomerAthlete</t>
+  </si>
+  <si>
+    <t>CustomerCountry</t>
+  </si>
+  <si>
+    <t>ModalityAthlete</t>
+  </si>
+  <si>
+    <t>TicketEventCompetitionEvent</t>
+  </si>
+  <si>
+    <t>ModalityCustomer</t>
+  </si>
+  <si>
+    <t>SportCustomer</t>
+  </si>
+  <si>
+    <t>Entities</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Mapping</t>
+  </si>
+  <si>
+    <t>CodeFirst</t>
+  </si>
+  <si>
+    <t>FirstMig</t>
+  </si>
+  <si>
+    <t>SecMig</t>
+  </si>
+  <si>
+    <t>Migration</t>
+  </si>
+  <si>
+    <t>SeedDB</t>
+  </si>
+  <si>
+    <t>Rio de Janeiro</t>
+  </si>
+  <si>
+    <t>07/08/2016 - 09:00 - Swimming morning Multisession</t>
+  </si>
+  <si>
+    <t>06/08/2016 - 09:00 - Swimming morning multisession</t>
+  </si>
+  <si>
+    <t>13/08/2016 - 09:00 - Swimming morning multissesion</t>
   </si>
 </sst>
 </file>
@@ -554,7 +606,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -751,17 +803,6 @@
     </border>
     <border>
       <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -777,7 +818,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -824,6 +865,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -869,7 +913,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -894,6 +938,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1178,8 +1234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AD56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Y45" sqref="Y45"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1211,43 +1267,43 @@
     <col min="25" max="25" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="26.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="28"/>
-      <c r="M2" s="26" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" s="28"/>
-      <c r="Q2" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
-      <c r="Y2" s="27"/>
-      <c r="Z2" s="27"/>
-      <c r="AA2" s="27"/>
-      <c r="AB2" s="27"/>
-      <c r="AC2" s="27"/>
-      <c r="AD2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="29"/>
+      <c r="M2" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="29"/>
+      <c r="Q2" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" s="28"/>
+      <c r="S2" s="28"/>
+      <c r="T2" s="28"/>
+      <c r="U2" s="28"/>
+      <c r="V2" s="28"/>
+      <c r="W2" s="28"/>
+      <c r="X2" s="28"/>
+      <c r="Y2" s="28"/>
+      <c r="Z2" s="28"/>
+      <c r="AA2" s="28"/>
+      <c r="AB2" s="28"/>
+      <c r="AC2" s="28"/>
+      <c r="AD2" s="29"/>
     </row>
     <row r="3" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="13" t="s">
@@ -1262,21 +1318,21 @@
       <c r="F3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="26" t="s">
-        <v>38</v>
-      </c>
-      <c r="I3" s="28"/>
-      <c r="M3" s="37" t="s">
-        <v>156</v>
-      </c>
-      <c r="N3" s="38" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q3" s="35" t="s">
+      <c r="H3" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" s="29"/>
+      <c r="M3" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="N3" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="36" t="s">
         <v>1</v>
       </c>
       <c r="R3" s="13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="S3" s="13" t="s">
         <v>9</v>
@@ -1285,34 +1341,34 @@
         <v>10</v>
       </c>
       <c r="U3" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="V3" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="V3" s="36" t="s">
+      <c r="W3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="X3" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y3" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z3" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA3" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="W3" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="X3" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y3" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="Z3" s="13" t="s">
+      <c r="AB3" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="AA3" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB3" s="13" t="s">
+      <c r="AC3" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="AC3" s="13" t="s">
+      <c r="AD3" s="8" t="s">
         <v>29</v>
-      </c>
-      <c r="AD3" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="4" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1331,8 +1387,8 @@
       <c r="F4" s="7">
         <v>1</v>
       </c>
-      <c r="H4" s="35" t="s">
-        <v>35</v>
+      <c r="H4" s="36" t="s">
+        <v>34</v>
       </c>
       <c r="I4" s="8" t="s">
         <v>2</v>
@@ -1347,31 +1403,31 @@
         <v>1</v>
       </c>
       <c r="R4" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="S4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="S4" s="12" t="s">
+      <c r="T4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="T4" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="U4" s="12">
-        <v>34</v>
+      <c r="U4" s="19">
+        <v>30071</v>
       </c>
       <c r="V4" s="12">
         <v>1</v>
       </c>
       <c r="W4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="X4" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="X4" s="12" t="s">
+      <c r="Y4" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="Y4" s="12" t="s">
+      <c r="Z4" s="12" t="s">
         <v>41</v>
-      </c>
-      <c r="Z4" s="12" t="s">
-        <v>42</v>
       </c>
       <c r="AA4" s="12">
         <v>3</v>
@@ -1380,10 +1436,10 @@
         <v>2099</v>
       </c>
       <c r="AC4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="AD4" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="AD4" s="7" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="5" spans="2:30" x14ac:dyDescent="0.25">
@@ -1391,7 +1447,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="12">
         <v>2</v>
@@ -1406,7 +1462,7 @@
         <v>1</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M5" s="2">
         <v>1</v>
@@ -1418,31 +1474,31 @@
         <v>2</v>
       </c>
       <c r="R5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="S5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="T5" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="U5" s="17">
+        <v>21575</v>
+      </c>
+      <c r="V5" s="10">
+        <v>2</v>
+      </c>
+      <c r="W5" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="T5" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="U5" s="10">
-        <v>57</v>
-      </c>
-      <c r="V5" s="10">
-        <v>2</v>
-      </c>
-      <c r="W5" s="10" t="s">
+      <c r="X5" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="X5" s="10" t="s">
+      <c r="Y5" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="Y5" s="10" t="s">
+      <c r="Z5" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="Z5" s="10" t="s">
-        <v>50</v>
       </c>
       <c r="AA5" s="10">
         <v>1</v>
@@ -1451,10 +1507,10 @@
         <v>81280270</v>
       </c>
       <c r="AC5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="AD5" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="AD5" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="6" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1477,7 +1533,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M6" s="2">
         <v>2</v>
@@ -1489,31 +1545,31 @@
         <v>3</v>
       </c>
       <c r="R6" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="S6" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="T6" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="S6" s="11" t="s">
+      <c r="U6" s="18">
+        <v>28971</v>
+      </c>
+      <c r="V6" s="11">
+        <v>1</v>
+      </c>
+      <c r="W6" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="T6" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="U6" s="11">
-        <v>38</v>
-      </c>
-      <c r="V6" s="11">
-        <v>1</v>
-      </c>
-      <c r="W6" s="11" t="s">
+      <c r="X6" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y6" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="X6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y6" s="11" t="s">
+      <c r="Z6" s="11" t="s">
         <v>58</v>
-      </c>
-      <c r="Z6" s="11" t="s">
-        <v>59</v>
       </c>
       <c r="AA6" s="11">
         <v>4</v>
@@ -1522,10 +1578,10 @@
         <v>43000</v>
       </c>
       <c r="AC6" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AD6" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1533,7 +1589,7 @@
         <v>4</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D7" s="11">
         <v>0</v>
@@ -1553,51 +1609,51 @@
     </row>
     <row r="8" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="M9" s="26" t="s">
-        <v>145</v>
-      </c>
-      <c r="N9" s="28"/>
-      <c r="Q9" s="26" t="s">
-        <v>65</v>
-      </c>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="28"/>
+      <c r="M9" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="N9" s="29"/>
+      <c r="Q9" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="R9" s="28"/>
+      <c r="S9" s="28"/>
+      <c r="T9" s="29"/>
     </row>
     <row r="10" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27"/>
-      <c r="K10" s="28"/>
-      <c r="M10" s="37" t="s">
-        <v>156</v>
-      </c>
-      <c r="N10" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="Q10" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="R10" s="36" t="s">
-        <v>156</v>
+      <c r="B10" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
+      <c r="M10" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="N10" s="39" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q10" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="R10" s="37" t="s">
+        <v>155</v>
       </c>
       <c r="S10" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="T10" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="T10" s="9" t="s">
-        <v>64</v>
-      </c>
     </row>
     <row r="11" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="35" t="s">
+      <c r="B11" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="14" t="s">
@@ -1610,13 +1666,13 @@
         <v>10</v>
       </c>
       <c r="F11" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="G11" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="H11" s="37" t="s">
         <v>12</v>
-      </c>
-      <c r="H11" s="36" t="s">
-        <v>13</v>
       </c>
       <c r="I11" s="14" t="s">
         <v>5</v>
@@ -1639,12 +1695,12 @@
       <c r="R11" s="12">
         <v>1</v>
       </c>
-      <c r="S11" s="18">
+      <c r="S11" s="19">
         <v>42495</v>
       </c>
       <c r="T11" s="7">
         <f>U19+U20+U21</f>
-        <v>2476.5</v>
+        <v>1676.5</v>
       </c>
     </row>
     <row r="12" spans="2:30" x14ac:dyDescent="0.25">
@@ -1652,16 +1708,16 @@
         <v>1</v>
       </c>
       <c r="C12" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>153</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="12">
-        <v>25</v>
+      <c r="F12" s="19">
+        <v>33010</v>
       </c>
       <c r="G12" s="12">
         <v>1</v>
@@ -1690,12 +1746,12 @@
       <c r="R12" s="10">
         <v>2</v>
       </c>
-      <c r="S12" s="16">
+      <c r="S12" s="17">
         <v>42498</v>
       </c>
       <c r="T12" s="3">
-        <f>U22</f>
-        <v>2160</v>
+        <f>U22+U24</f>
+        <v>1096.5</v>
       </c>
     </row>
     <row r="13" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1703,16 +1759,16 @@
         <v>2</v>
       </c>
       <c r="C13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="E13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="10">
-        <v>28</v>
+      <c r="F13" s="17">
+        <v>31588</v>
       </c>
       <c r="G13" s="10">
         <v>1</v>
@@ -1741,12 +1797,12 @@
       <c r="R13" s="11">
         <v>3</v>
       </c>
-      <c r="S13" s="17">
-        <v>42501</v>
+      <c r="S13" s="18">
+        <v>42503</v>
       </c>
       <c r="T13" s="5">
         <f>U23</f>
-        <v>1008</v>
+        <v>882</v>
       </c>
     </row>
     <row r="14" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1754,16 +1810,16 @@
         <v>3</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="F14" s="10">
-        <v>34</v>
+        <v>158</v>
+      </c>
+      <c r="F14" s="17">
+        <v>30561</v>
       </c>
       <c r="G14" s="10">
         <v>1</v>
@@ -1792,16 +1848,16 @@
         <v>4</v>
       </c>
       <c r="C15" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="11" t="s">
-        <v>154</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="11">
-        <v>24</v>
+      <c r="F15" s="41">
+        <v>32726</v>
       </c>
       <c r="G15" s="11">
         <v>1</v>
@@ -1821,69 +1877,69 @@
     </row>
     <row r="16" spans="2:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="17" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="C17" s="28"/>
-      <c r="E17" s="26" t="s">
+      <c r="B17" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="E17" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="F17" s="29"/>
+      <c r="H17" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="H17" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" s="28"/>
-      <c r="M17" s="26" t="s">
+      <c r="I17" s="29"/>
+      <c r="M17" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="N17" s="29"/>
+      <c r="Q17" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="R17" s="28"/>
+      <c r="S17" s="28"/>
+      <c r="T17" s="28"/>
+      <c r="U17" s="29"/>
+    </row>
+    <row r="18" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="38" t="s">
+        <v>75</v>
+      </c>
+      <c r="F18" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="H18" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M18" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="N18" s="39" t="s">
         <v>77</v>
       </c>
-      <c r="N17" s="28"/>
-      <c r="Q17" s="29" t="s">
+      <c r="Q18" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="R17" s="30"/>
-      <c r="S17" s="30"/>
-      <c r="T17" s="30"/>
-      <c r="U17" s="31"/>
-    </row>
-    <row r="18" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="E18" s="37" t="s">
-        <v>76</v>
-      </c>
-      <c r="F18" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="H18" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M18" s="37" t="s">
-        <v>156</v>
-      </c>
-      <c r="N18" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="Q18" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="R18" s="36" t="s">
-        <v>70</v>
-      </c>
-      <c r="S18" s="36" t="s">
+      <c r="S18" s="37" t="s">
+        <v>65</v>
+      </c>
+      <c r="T18" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="T18" s="14" t="s">
+      <c r="U18" s="15" t="s">
         <v>67</v>
-      </c>
-      <c r="U18" s="15" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
@@ -1891,7 +1947,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E19" s="6">
         <v>1</v>
@@ -1903,7 +1959,7 @@
         <v>1</v>
       </c>
       <c r="I19" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="M19" s="6">
         <v>1</v>
@@ -1924,7 +1980,7 @@
         <v>3</v>
       </c>
       <c r="U19" s="7">
-        <f>S27*T19</f>
+        <f>S29*T19</f>
         <v>136.5</v>
       </c>
     </row>
@@ -1933,7 +1989,7 @@
         <v>2</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E20" s="2">
         <v>2</v>
@@ -1945,7 +2001,7 @@
         <v>2</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="M20" s="2">
         <v>1</v>
@@ -1966,7 +2022,7 @@
         <v>5</v>
       </c>
       <c r="U20" s="3">
-        <f>S28*T20</f>
+        <f>S30*T20</f>
         <v>900</v>
       </c>
     </row>
@@ -1975,10 +2031,10 @@
         <v>3</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F21" s="3">
         <v>1</v>
@@ -2002,8 +2058,8 @@
         <v>4</v>
       </c>
       <c r="U21" s="3">
-        <f>S29*T21</f>
-        <v>1440</v>
+        <f>S31*T21</f>
+        <v>640</v>
       </c>
     </row>
     <row r="22" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2011,13 +2067,13 @@
         <v>4</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="E22" s="4">
-        <v>3</v>
-      </c>
-      <c r="F22" s="5">
-        <v>3</v>
+        <v>84</v>
+      </c>
+      <c r="E22" s="2">
+        <v>3</v>
+      </c>
+      <c r="F22" s="3">
+        <v>4</v>
       </c>
       <c r="M22" s="4">
         <v>3</v>
@@ -2038,239 +2094,246 @@
         <v>8</v>
       </c>
       <c r="U22" s="3">
-        <f>S30*T22</f>
-        <v>2160</v>
+        <f>S32*T22</f>
+        <v>960</v>
       </c>
     </row>
     <row r="23" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q23" s="4">
+      <c r="E23" s="4">
+        <v>4</v>
+      </c>
+      <c r="F23" s="5">
+        <v>3</v>
+      </c>
+      <c r="Q23" s="2">
         <v>5</v>
       </c>
-      <c r="R23" s="11">
+      <c r="R23" s="10">
         <v>5</v>
       </c>
-      <c r="S23" s="11">
-        <v>3</v>
-      </c>
-      <c r="T23" s="11">
+      <c r="S23" s="10">
+        <v>3</v>
+      </c>
+      <c r="T23" s="10">
         <v>7</v>
       </c>
-      <c r="U23" s="5">
-        <f>S31*T23</f>
-        <v>1008</v>
-      </c>
-    </row>
-    <row r="24" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="U23" s="3">
+        <f>S33*T23</f>
+        <v>882</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="Q24" s="2">
+        <v>6</v>
+      </c>
+      <c r="R24" s="10">
+        <v>2</v>
+      </c>
+      <c r="S24" s="10">
+        <v>2</v>
+      </c>
+      <c r="T24" s="10">
+        <v>3</v>
+      </c>
+      <c r="U24" s="3">
+        <f>S29*T24</f>
+        <v>136.5</v>
+      </c>
+    </row>
     <row r="25" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="26" t="s">
+      <c r="B25" s="27" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="29"/>
+      <c r="G25" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="H25" s="29"/>
+      <c r="J25" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="K25" s="29"/>
+      <c r="Q25" s="4">
+        <v>7</v>
+      </c>
+      <c r="R25" s="11">
+        <v>6</v>
+      </c>
+      <c r="S25" s="11">
+        <v>3</v>
+      </c>
+      <c r="T25" s="11">
+        <v>3</v>
+      </c>
+      <c r="U25" s="5">
+        <f>S34*T25</f>
+        <v>360</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D26" s="37" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="27"/>
-      <c r="D25" s="27"/>
-      <c r="E25" s="28"/>
-      <c r="G25" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="H25" s="28"/>
-      <c r="J25" s="26" t="s">
-        <v>99</v>
-      </c>
-      <c r="K25" s="28"/>
-      <c r="Q25" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="R25" s="30"/>
-      <c r="S25" s="30"/>
-      <c r="T25" s="30"/>
-      <c r="U25" s="31"/>
-    </row>
-    <row r="26" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D26" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="40" t="s">
+        <v>77</v>
+      </c>
+      <c r="G26" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="K26" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="M26" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="G26" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="J26" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="K26" s="9" t="s">
-        <v>2</v>
-      </c>
-      <c r="M26" s="29" t="s">
-        <v>79</v>
-      </c>
       <c r="N26" s="31"/>
-      <c r="Q26" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="R26" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="S26" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="T26" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="U26" s="39" t="s">
-        <v>74</v>
-      </c>
     </row>
     <row r="27" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6">
         <v>1</v>
       </c>
       <c r="C27" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="D27" s="12">
+        <v>1</v>
+      </c>
+      <c r="E27" s="7">
+        <v>1</v>
+      </c>
+      <c r="G27" s="6">
+        <v>1</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="J27" s="6">
+        <v>1</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="M27" s="38" t="s">
+        <v>155</v>
+      </c>
+      <c r="N27" s="39" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q27" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="R27" s="28"/>
+      <c r="S27" s="28"/>
+      <c r="T27" s="28"/>
+      <c r="U27" s="29"/>
+    </row>
+    <row r="28" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="2">
+        <v>2</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="D27" s="12">
-        <v>1</v>
-      </c>
-      <c r="E27" s="7">
-        <v>1</v>
-      </c>
-      <c r="G27" s="6">
-        <v>1</v>
-      </c>
-      <c r="H27" s="7" t="s">
-        <v>144</v>
-      </c>
-      <c r="J27" s="6">
-        <v>1</v>
-      </c>
-      <c r="K27" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="M27" s="37" t="s">
-        <v>156</v>
-      </c>
-      <c r="N27" s="38" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q27" s="6">
-        <v>1</v>
-      </c>
-      <c r="R27" s="25" t="s">
-        <v>155</v>
-      </c>
-      <c r="S27" s="12">
+      <c r="D28" s="10">
+        <v>1</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="G28" s="2">
+        <v>2</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="J28" s="2">
+        <v>2</v>
+      </c>
+      <c r="K28" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="M28" s="6">
+        <v>1</v>
+      </c>
+      <c r="N28" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q28" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="R28" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="S28" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="T28" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="U28" s="40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>3</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="D29" s="10">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="G29" s="2">
+        <v>3</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="J29" s="2">
+        <v>3</v>
+      </c>
+      <c r="K29" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="M29" s="2">
+        <v>1</v>
+      </c>
+      <c r="N29" s="3">
+        <v>7</v>
+      </c>
+      <c r="Q29" s="6">
+        <v>1</v>
+      </c>
+      <c r="R29" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="S29" s="43">
         <f>O47*D49</f>
         <v>45.5</v>
       </c>
-      <c r="T27" s="12">
-        <v>19997</v>
-      </c>
-      <c r="U27" s="7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B28" s="2">
-        <v>2</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="10">
-        <v>1</v>
-      </c>
-      <c r="E28" s="3">
-        <v>1</v>
-      </c>
-      <c r="G28" s="2">
-        <v>2</v>
-      </c>
-      <c r="H28" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="J28" s="2">
-        <v>2</v>
-      </c>
-      <c r="K28" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="M28" s="6">
-        <v>1</v>
-      </c>
-      <c r="N28" s="7">
-        <v>1</v>
-      </c>
-      <c r="Q28" s="2">
-        <v>2</v>
-      </c>
-      <c r="R28" s="33" t="s">
-        <v>157</v>
-      </c>
-      <c r="S28" s="32">
-        <f>O48*D50</f>
-        <v>180</v>
-      </c>
-      <c r="T28" s="10">
-        <v>19995</v>
-      </c>
-      <c r="U28" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B29" s="2">
-        <v>3</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="D29" s="10">
-        <v>2</v>
-      </c>
-      <c r="E29" s="3">
-        <v>1</v>
-      </c>
-      <c r="G29" s="2">
-        <v>3</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="J29" s="2">
-        <v>3</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="M29" s="2">
-        <v>1</v>
-      </c>
-      <c r="N29" s="3">
-        <v>7</v>
-      </c>
-      <c r="Q29" s="2">
-        <v>3</v>
-      </c>
-      <c r="R29" s="33" t="s">
-        <v>158</v>
-      </c>
-      <c r="S29" s="10">
-        <f>O54*D54</f>
-        <v>360</v>
-      </c>
-      <c r="T29" s="10">
-        <v>19996</v>
-      </c>
-      <c r="U29" s="3">
-        <v>7</v>
+      <c r="T29" s="12">
+        <v>1994</v>
+      </c>
+      <c r="U29" s="7">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="2:21" x14ac:dyDescent="0.25">
@@ -2278,7 +2341,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D30" s="10">
         <v>1</v>
@@ -2290,13 +2353,13 @@
         <v>4</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J30" s="2">
         <v>4</v>
       </c>
       <c r="K30" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="M30" s="2">
         <v>2</v>
@@ -2305,20 +2368,19 @@
         <v>3</v>
       </c>
       <c r="Q30" s="2">
-        <v>4</v>
-      </c>
-      <c r="R30" s="33" t="s">
-        <v>161</v>
-      </c>
-      <c r="S30" s="10">
-        <f>O56*D53</f>
-        <v>270</v>
+        <v>2</v>
+      </c>
+      <c r="R30" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="S30" s="33">
+        <v>180</v>
       </c>
       <c r="T30" s="10">
-        <v>19992</v>
+        <v>1995</v>
       </c>
       <c r="U30" s="3">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2326,7 +2388,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D31" s="10">
         <v>2</v>
@@ -2338,13 +2400,13 @@
         <v>5</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J31" s="2">
         <v>5</v>
       </c>
       <c r="K31" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M31" s="4">
         <v>3</v>
@@ -2352,21 +2414,21 @@
       <c r="N31" s="5">
         <v>4</v>
       </c>
-      <c r="Q31" s="4">
-        <v>5</v>
+      <c r="Q31" s="2">
+        <v>3</v>
       </c>
       <c r="R31" s="34" t="s">
-        <v>162</v>
-      </c>
-      <c r="S31" s="11">
-        <f>O55*D56</f>
-        <v>144</v>
-      </c>
-      <c r="T31" s="11">
-        <v>19993</v>
-      </c>
-      <c r="U31" s="5">
-        <v>9</v>
+        <v>177</v>
+      </c>
+      <c r="S31" s="33">
+        <f>O54*D54</f>
+        <v>160</v>
+      </c>
+      <c r="T31" s="10">
+        <v>1996</v>
+      </c>
+      <c r="U31" s="3">
+        <v>7</v>
       </c>
     </row>
     <row r="32" spans="2:21" x14ac:dyDescent="0.25">
@@ -2374,7 +2436,7 @@
         <v>6</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D32" s="10">
         <v>1</v>
@@ -2386,21 +2448,37 @@
         <v>6</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J32" s="2">
         <v>6</v>
       </c>
       <c r="K32" s="3" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>108</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>4</v>
+      </c>
+      <c r="R32" s="34" t="s">
+        <v>179</v>
+      </c>
+      <c r="S32" s="33">
+        <f>O56*D53</f>
+        <v>120</v>
+      </c>
+      <c r="T32" s="10">
+        <v>1992</v>
+      </c>
+      <c r="U32" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="4">
         <v>7</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D33" s="11">
         <v>2</v>
@@ -2412,65 +2490,97 @@
         <v>7</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J33" s="2">
         <v>7</v>
       </c>
       <c r="K33" s="3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>5</v>
+      </c>
+      <c r="R33" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="S33" s="33">
+        <f>O55*D56</f>
+        <v>126</v>
+      </c>
+      <c r="T33" s="10">
+        <v>1993</v>
+      </c>
+      <c r="U33" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G34" s="2">
         <v>8</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J34" s="2">
         <v>8</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="M34" s="26" t="s">
-        <v>128</v>
-      </c>
-      <c r="N34" s="28"/>
-    </row>
-    <row r="35" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="M34" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="N34" s="29"/>
+      <c r="Q34" s="4">
+        <v>6</v>
+      </c>
+      <c r="R34" s="35" t="s">
+        <v>178</v>
+      </c>
+      <c r="S34" s="44">
+        <f>O49*D53</f>
+        <v>120</v>
+      </c>
+      <c r="T34" s="11">
+        <v>1994</v>
+      </c>
+      <c r="U34" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G35" s="2">
         <v>9</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J35" s="2">
         <v>9</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="M35" s="37" t="s">
-        <v>129</v>
-      </c>
-      <c r="N35" s="38" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="36" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+      <c r="M35" s="38" t="s">
+        <v>128</v>
+      </c>
+      <c r="N35" s="39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="36" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G36" s="4">
         <v>10</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J36" s="4">
         <v>10</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="M36" s="6">
         <v>1</v>
@@ -2479,7 +2589,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="M37" s="2">
         <v>2</v>
       </c>
@@ -2487,15 +2597,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="26" t="s">
-        <v>114</v>
-      </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
+    <row r="38" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="28"/>
+      <c r="D38" s="28"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="28"/>
       <c r="G38" s="28"/>
+      <c r="H38" s="29"/>
       <c r="M38" s="2">
         <v>8</v>
       </c>
@@ -2503,23 +2614,26 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B39" s="35" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D39" s="13" t="s">
-        <v>113</v>
-      </c>
-      <c r="E39" s="13" t="s">
+    <row r="39" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B39" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="E39" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="F39" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="F39" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="G39" s="9" t="s">
+      <c r="G39" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H39" s="15" t="s">
         <v>27</v>
       </c>
       <c r="M39" s="2">
@@ -2529,157 +2643,187 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B40" s="6">
         <v>1</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D40" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="G40" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="H40" s="7">
+        <v>64585269</v>
+      </c>
+      <c r="M40" s="2">
+        <v>9</v>
+      </c>
+      <c r="N40" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B41" s="2">
+        <v>2</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E40" s="12" t="s">
+      <c r="E41" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="F40" s="12">
-        <v>64585269</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="M40" s="4">
-        <v>9</v>
-      </c>
-      <c r="N40" s="5">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B41" s="2">
-        <v>2</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D41" s="10" t="s">
+      <c r="F41" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H41" s="3">
+        <v>63348684</v>
+      </c>
+      <c r="M41" s="2">
+        <v>3</v>
+      </c>
+      <c r="N41" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B42" s="2">
+        <v>3</v>
+      </c>
+      <c r="C42" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="E41" s="10" t="s">
+      <c r="E42" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="F41" s="10">
-        <v>63348684</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
-      <c r="B42" s="2">
-        <v>3</v>
-      </c>
-      <c r="C42" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="E42" s="10" t="s">
-        <v>121</v>
-      </c>
-      <c r="F42" s="10">
+      <c r="F42" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="H42" s="3">
         <v>69484131</v>
       </c>
-      <c r="G42" s="3" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="43" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M42" s="2">
+        <v>4</v>
+      </c>
+      <c r="N42" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="43" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="4">
         <v>4</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E43" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="G43" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="F43" s="11">
+      <c r="H43" s="5">
         <v>63215987</v>
       </c>
-      <c r="G43" s="5" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="45" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H45" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="I45" s="27"/>
-      <c r="J45" s="27"/>
-      <c r="K45" s="27"/>
-      <c r="L45" s="27"/>
-      <c r="M45" s="27"/>
-      <c r="N45" s="27"/>
-      <c r="O45" s="28"/>
-    </row>
-    <row r="46" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="26" t="s">
-        <v>147</v>
-      </c>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="28"/>
-      <c r="H46" s="35" t="s">
+      <c r="M43" s="4">
+        <v>5</v>
+      </c>
+      <c r="N43" s="5">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="45" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H45" s="27" t="s">
+        <v>133</v>
+      </c>
+      <c r="I45" s="28"/>
+      <c r="J45" s="28"/>
+      <c r="K45" s="28"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="28"/>
+      <c r="N45" s="28"/>
+      <c r="O45" s="29"/>
+    </row>
+    <row r="46" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B46" s="27" t="s">
+        <v>146</v>
+      </c>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28"/>
+      <c r="E46" s="29"/>
+      <c r="H46" s="36" t="s">
         <v>1</v>
       </c>
       <c r="I46" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="J46" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="J46" s="13" t="s">
-        <v>112</v>
-      </c>
-      <c r="K46" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="L46" s="36" t="s">
+      <c r="K46" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="L46" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="M46" s="37" t="s">
         <v>130</v>
       </c>
-      <c r="M46" s="36" t="s">
+      <c r="N46" s="37" t="s">
         <v>131</v>
       </c>
-      <c r="N46" s="36" t="s">
+      <c r="O46" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="O46" s="9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="47" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B47" s="35" t="s">
+    </row>
+    <row r="47" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="36" t="s">
         <v>1</v>
       </c>
       <c r="C47" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D47" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="E47" s="39" t="s">
-        <v>132</v>
+        <v>145</v>
+      </c>
+      <c r="E47" s="40" t="s">
+        <v>131</v>
       </c>
       <c r="H47" s="6">
         <v>1</v>
       </c>
-      <c r="I47" s="18">
+      <c r="I47" s="19">
         <v>42588</v>
       </c>
-      <c r="J47" s="23">
+      <c r="J47" s="24">
         <v>0.58333333333333337</v>
       </c>
       <c r="K47" s="12">
@@ -2694,16 +2838,16 @@
       <c r="N47" s="12">
         <v>2</v>
       </c>
-      <c r="O47" s="24">
+      <c r="O47" s="25">
         <v>35</v>
       </c>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B48" s="6">
         <v>1</v>
       </c>
       <c r="C48" s="12" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D48" s="12">
         <v>1</v>
@@ -2714,10 +2858,10 @@
       <c r="H48" s="2">
         <v>2</v>
       </c>
-      <c r="I48" s="16">
+      <c r="I48" s="17">
         <v>42603</v>
       </c>
-      <c r="J48" s="19">
+      <c r="J48" s="20">
         <v>0.625</v>
       </c>
       <c r="K48" s="10">
@@ -2732,7 +2876,7 @@
       <c r="N48" s="10">
         <v>2</v>
       </c>
-      <c r="O48" s="20">
+      <c r="O48" s="21">
         <v>120</v>
       </c>
     </row>
@@ -2741,7 +2885,7 @@
         <v>2</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D49" s="10">
         <v>1.3</v>
@@ -2752,10 +2896,10 @@
       <c r="H49" s="2">
         <v>3</v>
       </c>
-      <c r="I49" s="16">
+      <c r="I49" s="17">
         <v>42588</v>
       </c>
-      <c r="J49" s="19">
+      <c r="J49" s="20">
         <v>0.375</v>
       </c>
       <c r="K49" s="10">
@@ -2770,7 +2914,7 @@
       <c r="N49" s="10">
         <v>3</v>
       </c>
-      <c r="O49" s="20">
+      <c r="O49" s="21">
         <v>80</v>
       </c>
     </row>
@@ -2779,7 +2923,7 @@
         <v>3</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D50" s="10">
         <v>1.5</v>
@@ -2790,10 +2934,10 @@
       <c r="H50" s="2">
         <v>4</v>
       </c>
-      <c r="I50" s="16">
+      <c r="I50" s="17">
         <v>42588</v>
       </c>
-      <c r="J50" s="19">
+      <c r="J50" s="20">
         <v>0.3833333333333333</v>
       </c>
       <c r="K50" s="10">
@@ -2808,7 +2952,7 @@
       <c r="N50" s="10">
         <v>3</v>
       </c>
-      <c r="O50" s="20">
+      <c r="O50" s="21">
         <v>80</v>
       </c>
     </row>
@@ -2817,7 +2961,7 @@
         <v>4</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D51" s="10">
         <v>1.7</v>
@@ -2828,10 +2972,10 @@
       <c r="H51" s="2">
         <v>5</v>
       </c>
-      <c r="I51" s="16">
+      <c r="I51" s="17">
         <v>42588</v>
       </c>
-      <c r="J51" s="19">
+      <c r="J51" s="20">
         <v>0.39583333333333331</v>
       </c>
       <c r="K51" s="10">
@@ -2846,7 +2990,7 @@
       <c r="N51" s="10">
         <v>3</v>
       </c>
-      <c r="O51" s="20">
+      <c r="O51" s="21">
         <v>80</v>
       </c>
     </row>
@@ -2855,7 +2999,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D52" s="10">
         <v>1</v>
@@ -2866,10 +3010,10 @@
       <c r="H52" s="2">
         <v>6</v>
       </c>
-      <c r="I52" s="16">
+      <c r="I52" s="17">
         <v>42588</v>
       </c>
-      <c r="J52" s="19">
+      <c r="J52" s="20">
         <v>0.66666666666666663</v>
       </c>
       <c r="K52" s="10">
@@ -2884,8 +3028,8 @@
       <c r="N52" s="10">
         <v>3</v>
       </c>
-      <c r="O52" s="20">
-        <v>140</v>
+      <c r="O52" s="21">
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="2:15" x14ac:dyDescent="0.25">
@@ -2893,7 +3037,7 @@
         <v>6</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D53" s="10">
         <v>1.5</v>
@@ -2904,10 +3048,10 @@
       <c r="H53" s="2">
         <v>7</v>
       </c>
-      <c r="I53" s="16">
+      <c r="I53" s="17">
         <v>42588</v>
       </c>
-      <c r="J53" s="19">
+      <c r="J53" s="20">
         <v>0.67499999999999993</v>
       </c>
       <c r="K53" s="10">
@@ -2922,8 +3066,8 @@
       <c r="N53" s="10">
         <v>3</v>
       </c>
-      <c r="O53" s="20">
-        <v>140</v>
+      <c r="O53" s="21">
+        <v>80</v>
       </c>
     </row>
     <row r="54" spans="2:15" x14ac:dyDescent="0.25">
@@ -2931,7 +3075,7 @@
         <v>7</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D54" s="10">
         <v>2</v>
@@ -2942,10 +3086,10 @@
       <c r="H54" s="2">
         <v>8</v>
       </c>
-      <c r="I54" s="16">
+      <c r="I54" s="17">
         <v>42589</v>
       </c>
-      <c r="J54" s="19">
+      <c r="J54" s="20">
         <v>0.45833333333333331</v>
       </c>
       <c r="K54" s="10">
@@ -2960,8 +3104,8 @@
       <c r="N54" s="10">
         <v>3</v>
       </c>
-      <c r="O54" s="20">
-        <v>180</v>
+      <c r="O54" s="21">
+        <v>80</v>
       </c>
     </row>
     <row r="55" spans="2:15" x14ac:dyDescent="0.25">
@@ -2969,7 +3113,7 @@
         <v>8</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D55" s="10">
         <v>1</v>
@@ -2980,10 +3124,10 @@
       <c r="H55" s="2">
         <v>9</v>
       </c>
-      <c r="I55" s="16">
+      <c r="I55" s="17">
         <v>42591</v>
       </c>
-      <c r="J55" s="19">
+      <c r="J55" s="20">
         <v>0.41666666666666669</v>
       </c>
       <c r="K55" s="10">
@@ -2998,8 +3142,8 @@
       <c r="N55" s="10">
         <v>4</v>
       </c>
-      <c r="O55" s="20">
-        <v>80</v>
+      <c r="O55" s="21">
+        <v>70</v>
       </c>
     </row>
     <row r="56" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -3007,7 +3151,7 @@
         <v>9</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D56" s="11">
         <v>1.8</v>
@@ -3018,10 +3162,10 @@
       <c r="H56" s="4">
         <v>10</v>
       </c>
-      <c r="I56" s="17">
+      <c r="I56" s="18">
         <v>42595</v>
       </c>
-      <c r="J56" s="21">
+      <c r="J56" s="22">
         <v>0.45833333333333331</v>
       </c>
       <c r="K56" s="11">
@@ -3036,8 +3180,8 @@
       <c r="N56" s="11">
         <v>3</v>
       </c>
-      <c r="O56" s="22">
-        <v>180</v>
+      <c r="O56" s="23">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3045,6 +3189,7 @@
     <mergeCell ref="Q2:AD2"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="Q9:T9"/>
+    <mergeCell ref="B38:H38"/>
     <mergeCell ref="M9:N9"/>
     <mergeCell ref="M17:N17"/>
     <mergeCell ref="B2:F2"/>
@@ -3056,10 +3201,9 @@
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="Q17:U17"/>
     <mergeCell ref="B46:E46"/>
-    <mergeCell ref="Q25:U25"/>
+    <mergeCell ref="Q27:U27"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="J25:K25"/>
-    <mergeCell ref="B38:G38"/>
     <mergeCell ref="M34:N34"/>
     <mergeCell ref="H45:O45"/>
     <mergeCell ref="M26:N26"/>
@@ -3072,4 +3216,533 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:Q26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="17" width="9.140625" style="16"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C2" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="F2" s="32"/>
+    </row>
+    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="E3" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="F3" s="16" t="s">
+        <v>173</v>
+      </c>
+      <c r="G3" s="16" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="42" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="16">
+        <v>1</v>
+      </c>
+      <c r="D4" s="16">
+        <v>1</v>
+      </c>
+      <c r="E4" s="16">
+        <v>11</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0</v>
+      </c>
+      <c r="G4" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="42" t="s">
+        <v>133</v>
+      </c>
+      <c r="C5" s="16">
+        <v>1</v>
+      </c>
+      <c r="D5" s="16">
+        <v>1</v>
+      </c>
+      <c r="E5" s="16">
+        <v>1</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0</v>
+      </c>
+      <c r="G5" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="42" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" s="16">
+        <v>1</v>
+      </c>
+      <c r="D6" s="16">
+        <v>1</v>
+      </c>
+      <c r="E6" s="16">
+        <v>1</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0</v>
+      </c>
+      <c r="G6" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="42" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="16">
+        <v>1</v>
+      </c>
+      <c r="D7" s="16">
+        <v>1</v>
+      </c>
+      <c r="E7" s="16">
+        <v>1</v>
+      </c>
+      <c r="F7" s="16">
+        <v>0</v>
+      </c>
+      <c r="G7" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="16">
+        <v>1</v>
+      </c>
+      <c r="D8" s="16">
+        <v>1</v>
+      </c>
+      <c r="E8" s="16">
+        <v>1</v>
+      </c>
+      <c r="F8" s="16">
+        <v>0</v>
+      </c>
+      <c r="G8" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="42" t="s">
+        <v>161</v>
+      </c>
+      <c r="C9" s="16">
+        <v>1</v>
+      </c>
+      <c r="D9" s="16">
+        <v>1</v>
+      </c>
+      <c r="E9" s="16">
+        <v>1</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0</v>
+      </c>
+      <c r="G9" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="42" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="16">
+        <v>1</v>
+      </c>
+      <c r="D10" s="16">
+        <v>1</v>
+      </c>
+      <c r="E10" s="16">
+        <v>1</v>
+      </c>
+      <c r="F10" s="16">
+        <v>0</v>
+      </c>
+      <c r="G10" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="42" t="s">
+        <v>89</v>
+      </c>
+      <c r="C11" s="16">
+        <v>1</v>
+      </c>
+      <c r="D11" s="16">
+        <v>1</v>
+      </c>
+      <c r="E11" s="16">
+        <v>1</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0</v>
+      </c>
+      <c r="G11" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C12" s="16">
+        <v>1</v>
+      </c>
+      <c r="D12" s="16">
+        <v>1</v>
+      </c>
+      <c r="E12" s="16">
+        <v>1</v>
+      </c>
+      <c r="F12" s="16">
+        <v>0</v>
+      </c>
+      <c r="G12" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="16">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16">
+        <v>1</v>
+      </c>
+      <c r="E13" s="16">
+        <v>1</v>
+      </c>
+      <c r="F13" s="16">
+        <v>0</v>
+      </c>
+      <c r="G13" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="42" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="16">
+        <v>1</v>
+      </c>
+      <c r="D14" s="16">
+        <v>1</v>
+      </c>
+      <c r="E14" s="16">
+        <v>1</v>
+      </c>
+      <c r="F14" s="16">
+        <v>0</v>
+      </c>
+      <c r="G14" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="16">
+        <v>1</v>
+      </c>
+      <c r="D15" s="16">
+        <v>1</v>
+      </c>
+      <c r="E15" s="16">
+        <v>1</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="42" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="16">
+        <v>1</v>
+      </c>
+      <c r="D16" s="16">
+        <v>1</v>
+      </c>
+      <c r="E16" s="16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="16">
+        <v>0</v>
+      </c>
+      <c r="G16" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B17" s="42" t="s">
+        <v>113</v>
+      </c>
+      <c r="C17" s="16">
+        <v>1</v>
+      </c>
+      <c r="D17" s="16">
+        <v>1</v>
+      </c>
+      <c r="E17" s="16">
+        <v>1</v>
+      </c>
+      <c r="F17" s="16">
+        <v>0</v>
+      </c>
+      <c r="G17" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="C18" s="16">
+        <v>1</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1</v>
+      </c>
+      <c r="E18" s="16">
+        <v>1</v>
+      </c>
+      <c r="F18" s="16">
+        <v>0</v>
+      </c>
+      <c r="G18" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F20" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G20" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="42" t="s">
+        <v>162</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D21" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F21" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G21" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D22" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E22" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F22" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G22" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="42" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E23" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F23" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G23" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D24" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F24" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G24" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="42" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D25" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E25" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F25" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G25" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C26" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="E26" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="F26" s="16" t="s">
+        <v>153</v>
+      </c>
+      <c r="G26" s="16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C4">
+    <cfRule type="iconSet" priority="4">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D4:G4">
+    <cfRule type="iconSet" priority="3">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5:C26">
+    <cfRule type="iconSet" priority="2">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:G26">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols2" showValue="0">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="num" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
All changes to delivery to teacher
</commit_message>
<xml_diff>
--- a/OlympicGamesApp_Database.xlsx
+++ b/OlympicGamesApp_Database.xlsx
@@ -964,6 +964,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -982,7 +983,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1265,8 +1265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AF4" sqref="AF4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AE3" sqref="AE3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1305,35 +1305,35 @@
   <sheetData>
     <row r="1" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="44"/>
-      <c r="M2" s="42" t="s">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="45"/>
+      <c r="M2" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="44"/>
-      <c r="Q2" s="42" t="s">
+      <c r="N2" s="45"/>
+      <c r="Q2" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="43"/>
-      <c r="S2" s="43"/>
-      <c r="T2" s="43"/>
-      <c r="U2" s="43"/>
-      <c r="V2" s="43"/>
-      <c r="W2" s="43"/>
-      <c r="X2" s="43"/>
-      <c r="Y2" s="43"/>
-      <c r="Z2" s="43"/>
-      <c r="AA2" s="43"/>
-      <c r="AB2" s="43"/>
-      <c r="AC2" s="43"/>
-      <c r="AD2" s="43"/>
-      <c r="AE2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
+      <c r="Y2" s="44"/>
+      <c r="Z2" s="44"/>
+      <c r="AA2" s="44"/>
+      <c r="AB2" s="44"/>
+      <c r="AC2" s="44"/>
+      <c r="AD2" s="44"/>
+      <c r="AE2" s="45"/>
     </row>
     <row r="3" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="33" t="s">
@@ -1351,13 +1351,13 @@
       <c r="F3" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="J3" s="42" t="s">
+      <c r="J3" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="K3" s="44"/>
+      <c r="K3" s="45"/>
       <c r="M3" s="35" t="s">
         <v>154</v>
       </c>
@@ -1406,7 +1406,7 @@
       <c r="AD3" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="AE3" s="28" t="s">
+      <c r="AE3" s="37" t="s">
         <v>180</v>
       </c>
     </row>
@@ -1702,7 +1702,7 @@
       <c r="AB7" s="11">
         <v>2099</v>
       </c>
-      <c r="AC7" s="48" t="s">
+      <c r="AC7" s="42" t="s">
         <v>184</v>
       </c>
       <c r="AD7" s="11" t="s">
@@ -1714,31 +1714,31 @@
     </row>
     <row r="8" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q9" s="42" t="s">
+      <c r="Q9" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="R9" s="43"/>
-      <c r="S9" s="43"/>
-      <c r="T9" s="44"/>
+      <c r="R9" s="44"/>
+      <c r="S9" s="44"/>
+      <c r="T9" s="45"/>
     </row>
     <row r="10" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="42" t="s">
+      <c r="B10" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="43"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="43"/>
-      <c r="L10" s="44"/>
-      <c r="N10" s="42" t="s">
+      <c r="C10" s="44"/>
+      <c r="D10" s="44"/>
+      <c r="E10" s="44"/>
+      <c r="F10" s="44"/>
+      <c r="G10" s="44"/>
+      <c r="H10" s="44"/>
+      <c r="I10" s="44"/>
+      <c r="J10" s="44"/>
+      <c r="K10" s="44"/>
+      <c r="L10" s="45"/>
+      <c r="N10" s="43" t="s">
         <v>143</v>
       </c>
-      <c r="O10" s="44"/>
+      <c r="O10" s="45"/>
       <c r="Q10" s="33" t="s">
         <v>1</v>
       </c>
@@ -1783,7 +1783,7 @@
       <c r="K11" s="27" t="s">
         <v>7</v>
       </c>
-      <c r="L11" s="28" t="s">
+      <c r="L11" s="37" t="s">
         <v>180</v>
       </c>
       <c r="N11" s="35" t="s">
@@ -1997,34 +1997,34 @@
       </c>
     </row>
     <row r="16" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q16" s="42" t="s">
+      <c r="Q16" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="R16" s="43"/>
-      <c r="S16" s="43"/>
-      <c r="T16" s="43"/>
-      <c r="U16" s="43"/>
-      <c r="V16" s="44"/>
+      <c r="R16" s="44"/>
+      <c r="S16" s="44"/>
+      <c r="T16" s="44"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="45"/>
     </row>
     <row r="17" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="44"/>
-      <c r="G17" s="42" t="s">
+      <c r="C17" s="44"/>
+      <c r="D17" s="45"/>
+      <c r="G17" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="H17" s="44"/>
+      <c r="H17" s="45"/>
       <c r="I17" s="29"/>
-      <c r="J17" s="45" t="s">
+      <c r="J17" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="K17" s="46"/>
-      <c r="M17" s="42" t="s">
+      <c r="K17" s="47"/>
+      <c r="M17" s="43" t="s">
         <v>75</v>
       </c>
-      <c r="N17" s="44"/>
+      <c r="N17" s="45"/>
       <c r="Q17" s="33" t="s">
         <v>1</v>
       </c>
@@ -2051,7 +2051,7 @@
       <c r="C18" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="D18" s="28" t="s">
+      <c r="D18" s="37" t="s">
         <v>180</v>
       </c>
       <c r="G18" s="35" t="s">
@@ -2340,20 +2340,20 @@
       </c>
     </row>
     <row r="25" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="42" t="s">
+      <c r="B25" s="43" t="s">
         <v>88</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="44"/>
-      <c r="G25" s="42" t="s">
+      <c r="C25" s="44"/>
+      <c r="D25" s="44"/>
+      <c r="E25" s="45"/>
+      <c r="G25" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="H25" s="44"/>
-      <c r="J25" s="42" t="s">
+      <c r="H25" s="45"/>
+      <c r="J25" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="K25" s="44"/>
+      <c r="K25" s="45"/>
       <c r="Q25" s="4">
         <v>8</v>
       </c>
@@ -2400,10 +2400,10 @@
       <c r="K26" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="M26" s="45" t="s">
+      <c r="M26" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="N26" s="46"/>
+      <c r="N26" s="47"/>
     </row>
     <row r="27" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="6">
@@ -2436,13 +2436,13 @@
       <c r="N27" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="Q27" s="42" t="s">
+      <c r="Q27" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="R27" s="43"/>
-      <c r="S27" s="43"/>
-      <c r="T27" s="43"/>
-      <c r="U27" s="44"/>
+      <c r="R27" s="44"/>
+      <c r="S27" s="44"/>
+      <c r="T27" s="44"/>
+      <c r="U27" s="45"/>
     </row>
     <row r="28" spans="2:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2">
@@ -2732,10 +2732,10 @@
       <c r="K34" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="M34" s="42" t="s">
+      <c r="M34" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="N34" s="44"/>
+      <c r="N34" s="45"/>
       <c r="Q34" s="4">
         <v>6</v>
       </c>
@@ -2802,15 +2802,15 @@
       </c>
     </row>
     <row r="38" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B38" s="42" t="s">
+      <c r="B38" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43"/>
-      <c r="E38" s="43"/>
-      <c r="F38" s="43"/>
-      <c r="G38" s="43"/>
-      <c r="H38" s="44"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="44"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="44"/>
+      <c r="H38" s="45"/>
       <c r="M38" s="2">
         <v>8</v>
       </c>
@@ -2965,24 +2965,24 @@
     </row>
     <row r="44" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="45" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H45" s="42" t="s">
+      <c r="H45" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="I45" s="43"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="43"/>
-      <c r="L45" s="43"/>
-      <c r="M45" s="43"/>
-      <c r="N45" s="43"/>
-      <c r="O45" s="44"/>
+      <c r="I45" s="44"/>
+      <c r="J45" s="44"/>
+      <c r="K45" s="44"/>
+      <c r="L45" s="44"/>
+      <c r="M45" s="44"/>
+      <c r="N45" s="44"/>
+      <c r="O45" s="45"/>
     </row>
     <row r="46" spans="2:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B46" s="42" t="s">
+      <c r="B46" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="C46" s="43"/>
-      <c r="D46" s="43"/>
-      <c r="E46" s="44"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="45"/>
       <c r="H46" s="33" t="s">
         <v>1</v>
       </c>
@@ -3390,18 +3390,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B10:L10"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B46:E46"/>
-    <mergeCell ref="Q27:U27"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="M34:N34"/>
-    <mergeCell ref="H45:O45"/>
-    <mergeCell ref="M26:N26"/>
-    <mergeCell ref="J3:K3"/>
     <mergeCell ref="Q9:T9"/>
     <mergeCell ref="B38:H38"/>
     <mergeCell ref="N10:O10"/>
@@ -3411,6 +3399,18 @@
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="Q16:V16"/>
     <mergeCell ref="Q2:AE2"/>
+    <mergeCell ref="Q27:U27"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="J25:K25"/>
+    <mergeCell ref="M34:N34"/>
+    <mergeCell ref="H45:O45"/>
+    <mergeCell ref="M26:N26"/>
+    <mergeCell ref="B2:G2"/>
+    <mergeCell ref="B10:L10"/>
+    <mergeCell ref="J17:K17"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B46:E46"/>
+    <mergeCell ref="J3:K3"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="AC4" r:id="rId1"/>
@@ -3438,14 +3438,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="48" t="s">
         <v>170</v>
       </c>
-      <c r="D2" s="47"/>
-      <c r="E2" s="47" t="s">
+      <c r="D2" s="48"/>
+      <c r="E2" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="F2" s="47"/>
+      <c r="F2" s="48"/>
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">

</xml_diff>